<commit_message>
V1.1 -> Kleine index.html beigefügt + Daten auf Ch. 414 aktualisiert
</commit_message>
<xml_diff>
--- a/data/Characters_by_Appearance-RAW.xlsx
+++ b/data/Characters_by_Appearance-RAW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3987"/>
+  <dimension ref="A1:B3995"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -40305,6 +40305,86 @@
         </is>
       </c>
     </row>
+    <row r="3988">
+      <c r="A3988" t="n">
+        <v>414</v>
+      </c>
+      <c r="B3988" t="inlineStr">
+        <is>
+          <t>Shax Shakky</t>
+        </is>
+      </c>
+    </row>
+    <row r="3989">
+      <c r="A3989" t="n">
+        <v>414</v>
+      </c>
+      <c r="B3989" t="inlineStr">
+        <is>
+          <t>Malius Phantom /Andro M. Rock</t>
+        </is>
+      </c>
+    </row>
+    <row r="3990">
+      <c r="A3990" t="n">
+        <v>414</v>
+      </c>
+      <c r="B3990" t="inlineStr">
+        <is>
+          <t>Azazel Ameri</t>
+        </is>
+      </c>
+    </row>
+    <row r="3991">
+      <c r="A3991" t="n">
+        <v>414</v>
+      </c>
+      <c r="B3991" t="inlineStr">
+        <is>
+          <t>Muchara</t>
+        </is>
+      </c>
+    </row>
+    <row r="3992">
+      <c r="A3992" t="n">
+        <v>414</v>
+      </c>
+      <c r="B3992" t="inlineStr">
+        <is>
+          <t>Gamigin Ganjet</t>
+        </is>
+      </c>
+    </row>
+    <row r="3993">
+      <c r="A3993" t="n">
+        <v>414</v>
+      </c>
+      <c r="B3993" t="inlineStr">
+        <is>
+          <t>Andro M. Jazz(flashback)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3994">
+      <c r="A3994" t="n">
+        <v>414</v>
+      </c>
+      <c r="B3994" t="inlineStr">
+        <is>
+          <t>Iruma Suzuki</t>
+        </is>
+      </c>
+    </row>
+    <row r="3995">
+      <c r="A3995" t="n">
+        <v>414</v>
+      </c>
+      <c r="B3995" t="inlineStr">
+        <is>
+          <t>Arikured(flashback)</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>